<commit_message>
Logmsg function updated with manual wait through variable
</commit_message>
<xml_diff>
--- a/Data/Result/ResINSOR.xlsx
+++ b/Data/Result/ResINSOR.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>TestId</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>EAOR21AP-0315</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Folder Name updated and run execution in headless mode
</commit_message>
<xml_diff>
--- a/Data/Result/ResINSOR.xlsx
+++ b/Data/Result/ResINSOR.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>TestId</t>
   </si>
@@ -423,7 +423,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>

</xml_diff>